<commit_message>
Corrected values for T1
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.58333</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
@@ -490,13 +490,13 @@
         <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45384.56668242044</v>
+        <v>45385.3447201341</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45388.56668242044</v>
+        <v>45387.3447201341</v>
       </c>
     </row>
     <row r="3">
@@ -515,13 +515,13 @@
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>1.333333333333333</v>
+        <v>1.5</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45388.56668242044</v>
+        <v>45387.3447201341</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45389.56668242044</v>
+        <v>45389.3447201341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test 2 with file input
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -493,10 +493,10 @@
         <v>2</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45385.3447201341</v>
+        <v>45385.89280657649</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45387.3447201341</v>
+        <v>45387.89280657649</v>
       </c>
     </row>
     <row r="3">
@@ -518,10 +518,10 @@
         <v>1.5</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45387.3447201341</v>
+        <v>45387.89280657649</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45389.3447201341</v>
+        <v>45389.89280657649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>